<commit_message>
Répartition des cartes à jouer sur 100 cartes
</commit_message>
<xml_diff>
--- a/docs/Cartes-a-jouer--repartition.xlsx
+++ b/docs/Cartes-a-jouer--repartition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Documents\GitHub\Donjons-et-Barons\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2026ED4E-4805-4FE6-B3DE-5708903597A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23959BBA-AB7E-4AB3-AB0C-3EDE6D0538F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-9120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Type</t>
   </si>
@@ -135,6 +135,30 @@
   </si>
   <si>
     <t>Fréquence</t>
+  </si>
+  <si>
+    <t>Ordre</t>
+  </si>
+  <si>
+    <t>#Cartes Officier</t>
+  </si>
+  <si>
+    <t>#Cartes</t>
+  </si>
+  <si>
+    <t>#Cartes Troupes</t>
+  </si>
+  <si>
+    <t>#Cartes Déplacer Officiers</t>
+  </si>
+  <si>
+    <t>#Cartes Recruter Troupes</t>
+  </si>
+  <si>
+    <t>#Cartes Déplacer Troupes</t>
+  </si>
+  <si>
+    <t>#Cartes rares</t>
   </si>
 </sst>
 </file>
@@ -142,9 +166,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,13 +183,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBCDE5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -292,7 +342,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -321,13 +371,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -335,7 +406,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="21">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -439,10 +510,21 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
+        <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -527,6 +609,25 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -558,7 +659,37 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -573,38 +704,13 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEBCDE5"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -617,20 +723,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF687EBA-D301-4E43-8701-B804D42A43C7}" name="Tableau1" displayName="Tableau1" ref="B2:H18" totalsRowCount="1" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
-  <autoFilter ref="B2:H17" xr:uid="{CF687EBA-D301-4E43-8701-B804D42A43C7}"/>
-  <tableColumns count="7">
-    <tableColumn id="5" xr3:uid="{1ACE54E5-EDC8-4AD7-84A1-8DA8AE240D81}" name="Note" totalsRowFunction="count" dataDxfId="13" totalsRowDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{361935C2-34DD-4D21-A2AB-6BBFCF4F98A2}" name="Nombre" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{79576F61-0793-4990-BCCE-C22965121196}" name="Fréquence" dataDxfId="7" totalsRowDxfId="4" dataCellStyle="Pourcentage">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF687EBA-D301-4E43-8701-B804D42A43C7}" name="Tableau1" displayName="Tableau1" ref="B2:I18" totalsRowCount="1" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+  <autoFilter ref="B2:I17" xr:uid="{CF687EBA-D301-4E43-8701-B804D42A43C7}"/>
+  <tableColumns count="8">
+    <tableColumn id="5" xr3:uid="{1ACE54E5-EDC8-4AD7-84A1-8DA8AE240D81}" name="Note" totalsRowFunction="count" dataDxfId="15" totalsRowDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{962D52E2-C6AE-4100-AE8C-DF2E8B9B0615}" name="Ordre" dataDxfId="8" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{361935C2-34DD-4D21-A2AB-6BBFCF4F98A2}" name="Nombre" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{79576F61-0793-4990-BCCE-C22965121196}" name="Fréquence" dataDxfId="13" totalsRowDxfId="4" dataCellStyle="Pourcentage">
       <calculatedColumnFormula>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{37230C39-5DD0-41BC-BD2F-700C093E4770}" name="Nombre*Credit" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="3">
+    <tableColumn id="8" xr3:uid="{37230C39-5DD0-41BC-BD2F-700C093E4770}" name="Nombre*Credit" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="3">
       <calculatedColumnFormula>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{01749902-06D0-4021-B14B-C7F16B74E64F}" name="Rare?" dataDxfId="10" totalsRowDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{03B71102-410F-4504-A5D5-D6E86877D1E0}" name="Type" dataDxfId="9" totalsRowDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{D6FB2E1D-5A55-46E8-AE05-7C9175F7718F}" name="Credit" dataDxfId="8" totalsRowDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{01749902-06D0-4021-B14B-C7F16B74E64F}" name="Rare?" dataDxfId="11" totalsRowDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{03B71102-410F-4504-A5D5-D6E86877D1E0}" name="Type" dataDxfId="10" totalsRowDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{D6FB2E1D-5A55-46E8-AE05-7C9175F7718F}" name="Credit" dataDxfId="9" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -899,502 +1006,612 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:L33"/>
+  <dimension ref="B2:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="36.7109375" customWidth="1"/>
-    <col min="12" max="12" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="36.7109375" customWidth="1"/>
+    <col min="13" max="13" width="34.42578125" customWidth="1"/>
+    <col min="15" max="15" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
+      <c r="E3" s="11">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="1">
+        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>10</v>
+      </c>
+      <c r="E4" s="11">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="1">
+        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
+        <v>20</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>10</v>
+      </c>
+      <c r="E5" s="11">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="1">
+        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
+        <v>20</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>10</v>
+      </c>
+      <c r="E6" s="11">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="1">
+        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
+        <v>20</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="11">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
+        <v>0.02</v>
+      </c>
+      <c r="F7" s="1">
+        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
+        <v>4</v>
+      </c>
+      <c r="G7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1">
-        <v>4</v>
-      </c>
-      <c r="D3" s="11">
+      <c r="C8" s="2">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>3.125E-2</v>
-      </c>
-      <c r="E3" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="F8" s="1">
+        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="11">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
+        <v>0.02</v>
+      </c>
+      <c r="F9" s="1">
+        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
+        <v>6</v>
+      </c>
+      <c r="G9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1">
+        <v>12</v>
+      </c>
+      <c r="E10" s="11">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
+        <v>0.12</v>
+      </c>
+      <c r="F10" s="1">
         <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="b">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="3">
         <v>1</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1">
-        <v>4</v>
-      </c>
-      <c r="D4" s="11">
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1">
+        <v>8</v>
+      </c>
+      <c r="E11" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>3.125E-2</v>
-      </c>
-      <c r="E4" s="1">
-        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1">
-        <v>12</v>
-      </c>
-      <c r="D5" s="11">
-        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>9.375E-2</v>
-      </c>
-      <c r="E5" s="1">
-        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>24</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1">
-        <v>12</v>
-      </c>
-      <c r="D6" s="11">
-        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>9.375E-2</v>
-      </c>
-      <c r="E6" s="1">
-        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>24</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1">
-        <v>12</v>
-      </c>
-      <c r="D7" s="11">
-        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>9.375E-2</v>
-      </c>
-      <c r="E7" s="1">
-        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>24</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1">
-        <v>4</v>
-      </c>
-      <c r="D8" s="11">
-        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>3.125E-2</v>
-      </c>
-      <c r="E8" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="F11" s="1">
         <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
         <v>8</v>
       </c>
-      <c r="F8" s="1" t="b">
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="3">
         <v>1</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1">
-        <v>12</v>
-      </c>
-      <c r="D9" s="11">
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <v>8</v>
+      </c>
+      <c r="E12" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>9.375E-2</v>
-      </c>
-      <c r="E9" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="F12" s="1">
         <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="1">
         <v>8</v>
       </c>
-      <c r="D10" s="11">
-        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>6.25E-2</v>
-      </c>
-      <c r="E10" s="1">
-        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>24</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1" t="s">
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="1">
-        <v>8</v>
-      </c>
-      <c r="D11" s="11">
-        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>6.25E-2</v>
-      </c>
-      <c r="E11" s="1">
-        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>32</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="1">
-        <v>8</v>
-      </c>
-      <c r="D12" s="11">
-        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>6.25E-2</v>
-      </c>
-      <c r="E12" s="1">
-        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>40</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="1">
-        <v>8</v>
-      </c>
-      <c r="D13" s="11">
+      <c r="C13" s="2">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1">
+        <v>6</v>
+      </c>
+      <c r="E13" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>6.25E-2</v>
-      </c>
-      <c r="E13" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="F13" s="1">
         <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>8</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="3">
+      <c r="I13" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="1">
-        <v>10</v>
-      </c>
-      <c r="D14" s="11">
+        <v>18</v>
+      </c>
+      <c r="C14" s="2">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1">
+        <v>6</v>
+      </c>
+      <c r="E14" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>7.8125E-2</v>
-      </c>
-      <c r="E14" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="F14" s="1">
         <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>10</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H14" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="1">
-        <v>10</v>
-      </c>
-      <c r="D15" s="11">
+        <v>20</v>
+      </c>
+      <c r="C15" s="2">
+        <v>13</v>
+      </c>
+      <c r="D15" s="1">
+        <v>6</v>
+      </c>
+      <c r="E15" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>7.8125E-2</v>
-      </c>
-      <c r="E15" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="F15" s="1">
         <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>10</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="1">
-        <v>12</v>
-      </c>
-      <c r="D16" s="11">
+        <v>19</v>
+      </c>
+      <c r="C16" s="2">
+        <v>14</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6</v>
+      </c>
+      <c r="E16" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>9.375E-2</v>
-      </c>
-      <c r="E16" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="F16" s="1">
         <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>12</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H16" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I16" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
+        <v>15</v>
+      </c>
+      <c r="D17" s="8">
+        <v>2</v>
+      </c>
+      <c r="E17" s="12">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
+        <v>0.02</v>
+      </c>
+      <c r="F17" s="8">
+        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
+        <v>2</v>
+      </c>
+      <c r="G17" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="12">
-        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>3.125E-2</v>
-      </c>
-      <c r="E17" s="8">
-        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>4</v>
-      </c>
-      <c r="F17" s="8" t="b">
+      <c r="I17" s="9">
         <v>1</v>
       </c>
-      <c r="G17" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="H17" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
         <f>SUBTOTAL(103,Tableau1[Note])</f>
         <v>15</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="7"/>
+      <c r="D18" s="8">
         <f>SUBTOTAL(109,Tableau1[Nombre])</f>
-        <v>128</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8">
+        <v>100</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8">
         <f>SUBTOTAL(109,Tableau1[Nombre*Credit])</f>
-        <v>244</v>
-      </c>
-      <c r="F18" s="8"/>
+        <v>166</v>
+      </c>
       <c r="G18" s="8"/>
-      <c r="H18" s="9"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J20" s="1" t="s">
+      <c r="H18" s="8"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="1">
-        <v>50</v>
-      </c>
-      <c r="L21" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C21" s="13"/>
+      <c r="K21" s="1">
+        <v>40</v>
+      </c>
+      <c r="M21" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <f>Tableau1[[#Totals],[Nombre*Credit]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>1.90625</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J23" s="1" t="s">
+        <v>1.66</v>
+      </c>
+      <c r="C22" s="14"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="M23" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J24" s="1">
-        <f>ROUNDDOWN(J21/4,0)</f>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D24" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="K24" s="1">
+        <f>ROUNDDOWN(K21/4,0)</f>
+        <v>10</v>
+      </c>
+      <c r="M24" s="1">
+        <f>ROUNDUP(M21*0.6/4,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D25" s="15">
+        <f>4*M24</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K27" s="1">
+        <v>2</v>
+      </c>
+      <c r="M27" s="1">
+        <f>ROUNDDOWN(M21*0.4/2,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="18">
+        <f>4*K24</f>
+        <v>40</v>
+      </c>
+      <c r="D28" s="15">
+        <f>2*M27</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M29" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M30" s="1">
         <v>12</v>
       </c>
-      <c r="L24" s="1">
-        <f>ROUNDUP(L21*0.6/4,0)</f>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="18">
+        <f>4*K24+3*K27</f>
+        <v>46</v>
+      </c>
+      <c r="D31" s="15">
+        <f>4*M24+2*M27+M30+M33</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M32" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M33" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" s="16">
+        <f>B31+D31</f>
+        <v>100</v>
+      </c>
+      <c r="D34" s="1">
+        <f>3*K27+1*M33</f>
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J27" s="1">
-        <v>2</v>
-      </c>
-      <c r="L27" s="1">
-        <f>ROUNDDOWN(L21*0.4/2,0)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L29" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L30" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L32" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L33" s="1">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
Debut de production des cartes
</commit_message>
<xml_diff>
--- a/docs/Cartes-a-jouer--repartition.xlsx
+++ b/docs/Cartes-a-jouer--repartition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Documents\GitHub\Donjons-et-Barons\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A9B1CD-0836-40CD-9AE3-94D05F47262F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F10C2F-8DD9-4AAB-9BD1-90D93D736E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-9120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>Type</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>#Cartes rares</t>
+  </si>
+  <si>
+    <t>Prêt</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -385,7 +391,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="23">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -477,7 +483,9 @@
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -498,6 +506,38 @@
           <color indexed="64"/>
         </top>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -702,25 +742,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF687EBA-D301-4E43-8701-B804D42A43C7}" name="Tableau1" displayName="Tableau1" ref="B2:I18" totalsRowCount="1" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
-  <autoFilter ref="B2:I17" xr:uid="{CF687EBA-D301-4E43-8701-B804D42A43C7}">
-    <filterColumn colId="5">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
-  <tableColumns count="8">
-    <tableColumn id="5" xr3:uid="{1ACE54E5-EDC8-4AD7-84A1-8DA8AE240D81}" name="Note" totalsRowFunction="count" dataDxfId="15" totalsRowDxfId="7"/>
-    <tableColumn id="1" xr3:uid="{962D52E2-C6AE-4100-AE8C-DF2E8B9B0615}" name="Ordre" dataDxfId="14" totalsRowDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{361935C2-34DD-4D21-A2AB-6BBFCF4F98A2}" name="Nombre" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{79576F61-0793-4990-BCCE-C22965121196}" name="Fréquence" dataDxfId="12" totalsRowDxfId="4" dataCellStyle="Pourcentage">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF687EBA-D301-4E43-8701-B804D42A43C7}" name="Tableau1" displayName="Tableau1" ref="B2:J18" totalsRowCount="1" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+  <autoFilter ref="B2:J17" xr:uid="{CF687EBA-D301-4E43-8701-B804D42A43C7}"/>
+  <tableColumns count="9">
+    <tableColumn id="5" xr3:uid="{1ACE54E5-EDC8-4AD7-84A1-8DA8AE240D81}" name="Note" totalsRowFunction="count" dataDxfId="17" totalsRowDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{962D52E2-C6AE-4100-AE8C-DF2E8B9B0615}" name="Ordre" dataDxfId="16" totalsRowDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{361935C2-34DD-4D21-A2AB-6BBFCF4F98A2}" name="Nombre" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{C94B1093-5CDB-4631-9DEA-00E6458C936C}" name="Prêt" dataDxfId="9" totalsRowDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{79576F61-0793-4990-BCCE-C22965121196}" name="Fréquence" dataDxfId="14" totalsRowDxfId="4" dataCellStyle="Pourcentage">
       <calculatedColumnFormula>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{37230C39-5DD0-41BC-BD2F-700C093E4770}" name="Nombre*Credit" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="3">
+    <tableColumn id="8" xr3:uid="{37230C39-5DD0-41BC-BD2F-700C093E4770}" name="Nombre*Credit" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="3">
       <calculatedColumnFormula>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{01749902-06D0-4021-B14B-C7F16B74E64F}" name="Rare?" dataDxfId="10" totalsRowDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{03B71102-410F-4504-A5D5-D6E86877D1E0}" name="Type" dataDxfId="9" totalsRowDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{D6FB2E1D-5A55-46E8-AE05-7C9175F7718F}" name="Credit" dataDxfId="8" totalsRowDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{01749902-06D0-4021-B14B-C7F16B74E64F}" name="Rare?" dataDxfId="12" totalsRowDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{03B71102-410F-4504-A5D5-D6E86877D1E0}" name="Type" dataDxfId="11" totalsRowDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{D6FB2E1D-5A55-46E8-AE05-7C9175F7718F}" name="Credit" dataDxfId="10" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -989,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I34"/>
+  <dimension ref="B2:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N11" sqref="N10:N11"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,14 +1038,15 @@
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="7.28515625" customWidth="1"/>
     <col min="4" max="4" width="28.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="12" max="12" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1019,392 +1057,421 @@
         <v>5</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="11">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
+        <v>0.1</v>
+      </c>
+      <c r="G3" s="1">
+        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
+        <v>10</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D4" s="1">
         <v>9</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>9.7826086956521743E-2</v>
-      </c>
-      <c r="F3" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="G4" s="1">
         <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
         <v>0</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="3">
+      <c r="J4" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C5" s="2">
         <v>2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D5" s="1">
         <v>9</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>9.7826086956521743E-2</v>
-      </c>
-      <c r="F4" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="G5" s="1">
         <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
         <v>18</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1" t="s">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J5" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="2">
         <v>3</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D6" s="1">
         <v>9</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>9.7826086956521743E-2</v>
-      </c>
-      <c r="F5" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="G6" s="1">
         <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
         <v>18</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J6" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C7" s="2">
         <v>4</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D7" s="1">
         <v>9</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>9.7826086956521743E-2</v>
-      </c>
-      <c r="F6" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="G7" s="1">
         <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
         <v>18</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="3">
+      <c r="J7" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="11">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
+        <v>0.08</v>
+      </c>
+      <c r="G8" s="1">
+        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
+        <v>8</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2">
         <v>10</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D9" s="1">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="11">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
+        <v>0.08</v>
+      </c>
+      <c r="G9" s="1">
+        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
+        <v>8</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="11">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
+        <v>0.08</v>
+      </c>
+      <c r="G10" s="1">
+        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
+        <v>8</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="11">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
+        <v>0.08</v>
+      </c>
+      <c r="G11" s="1">
+        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
+        <v>24</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2">
+        <v>12</v>
+      </c>
+      <c r="D12" s="1">
+        <v>7</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="11">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G12" s="1">
+        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
+        <v>21</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2">
+        <v>13</v>
+      </c>
+      <c r="D13" s="1">
+        <v>7</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="11">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G13" s="1">
+        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
+        <v>21</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="2">
         <v>5</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D14" s="1">
         <v>2</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E14" s="1"/>
+      <c r="F14" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>2.1739130434782608E-2</v>
-      </c>
-      <c r="F7" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="G14" s="1">
         <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
         <v>4</v>
       </c>
-      <c r="G7" s="1" t="b">
+      <c r="H14" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="3">
+      <c r="J14" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C15" s="2">
         <v>6</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D15" s="1">
         <v>2</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E15" s="1"/>
+      <c r="F15" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>2.1739130434782608E-2</v>
-      </c>
-      <c r="F8" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="G15" s="1">
         <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
         <v>6</v>
       </c>
-      <c r="G8" s="1" t="b">
+      <c r="H15" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J15" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C16" s="2">
         <v>7</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D16" s="1">
         <v>2</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>2.1739130434782608E-2</v>
-      </c>
-      <c r="F9" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="G16" s="1">
         <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
         <v>6</v>
       </c>
-      <c r="G9" s="1" t="b">
+      <c r="H16" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J16" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2">
-        <v>8</v>
-      </c>
-      <c r="D10" s="1">
-        <v>10</v>
-      </c>
-      <c r="E10" s="11">
-        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>0.10869565217391304</v>
-      </c>
-      <c r="F10" s="1">
-        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>10</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="2">
-        <v>9</v>
-      </c>
-      <c r="D11" s="1">
-        <v>8</v>
-      </c>
-      <c r="E11" s="11">
-        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>8.6956521739130432E-2</v>
-      </c>
-      <c r="F11" s="1">
-        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>8</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="2">
-        <v>10</v>
-      </c>
-      <c r="D12" s="1">
-        <v>8</v>
-      </c>
-      <c r="E12" s="11">
-        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>8.6956521739130432E-2</v>
-      </c>
-      <c r="F12" s="1">
-        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>8</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I12" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="2">
-        <v>11</v>
-      </c>
-      <c r="D13" s="1">
-        <v>8</v>
-      </c>
-      <c r="E13" s="11">
-        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>8.6956521739130432E-2</v>
-      </c>
-      <c r="F13" s="1">
-        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>8</v>
-      </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I13" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="2">
-        <v>12</v>
-      </c>
-      <c r="D14" s="1">
-        <v>7</v>
-      </c>
-      <c r="E14" s="11">
-        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>7.6086956521739135E-2</v>
-      </c>
-      <c r="F14" s="1">
-        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>21</v>
-      </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I14" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="2">
-        <v>13</v>
-      </c>
-      <c r="D15" s="1">
-        <v>7</v>
-      </c>
-      <c r="E15" s="11">
-        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>7.6086956521739135E-2</v>
-      </c>
-      <c r="F15" s="1">
-        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>21</v>
-      </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I15" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="2">
-        <v>14</v>
-      </c>
-      <c r="D16" s="1">
-        <v>8</v>
-      </c>
-      <c r="E16" s="11">
-        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>8.6956521739130432E-2</v>
-      </c>
-      <c r="F16" s="1">
-        <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
-        <v>24</v>
-      </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>11</v>
       </c>
@@ -1414,44 +1481,46 @@
       <c r="D17" s="8">
         <v>2</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="8"/>
+      <c r="F17" s="12">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>2.1739130434782608E-2</v>
-      </c>
-      <c r="F17" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="G17" s="8">
         <f>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</f>
         <v>2</v>
       </c>
-      <c r="G17" s="8" t="b">
+      <c r="H17" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="I17" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I17" s="9">
+      <c r="J17" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
         <f>SUBTOTAL(103,Tableau1[Note])</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="8">
         <f>SUBTOTAL(109,Tableau1[Nombre])</f>
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E18" s="8"/>
-      <c r="F18" s="8">
+      <c r="F18" s="8"/>
+      <c r="G18" s="8">
         <f>SUBTOTAL(109,Tableau1[Nombre*Credit])</f>
-        <v>154</v>
-      </c>
-      <c r="G18" s="8"/>
+        <v>172</v>
+      </c>
       <c r="H18" s="8"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="8"/>
+      <c r="J18" s="9"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>24</v>
       </c>
@@ -1460,17 +1529,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <f>Tableau1[[#Totals],[Nombre*Credit]]/Tableau1[[#Totals],[Nombre]]</f>
-        <v>1.673913043478261</v>
+        <v>1.72</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="15">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>33</v>
       </c>
@@ -1478,7 +1547,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>8</v>
       </c>
@@ -1486,7 +1555,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="18" t="s">
         <v>30</v>
       </c>
@@ -1494,7 +1563,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="18">
         <v>36</v>
       </c>
@@ -1502,7 +1571,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="17" t="s">
         <v>27</v>
       </c>
@@ -1510,15 +1579,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="18">
         <v>42</v>
       </c>
       <c r="D31" s="15">
         <v>58</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Première version du jeu de cartes à joueur prête
</commit_message>
<xml_diff>
--- a/docs/Cartes-a-jouer--repartition.xlsx
+++ b/docs/Cartes-a-jouer--repartition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Documents\GitHub\Donjons-et-Barons\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F10C2F-8DD9-4AAB-9BD1-90D93D736E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1858DCC7-FF53-4340-86CB-564D5E5D7245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
   <si>
     <t>Type</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>z</t>
   </si>
 </sst>
 </file>
@@ -523,6 +526,56 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -541,56 +594,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -748,16 +751,16 @@
     <tableColumn id="5" xr3:uid="{1ACE54E5-EDC8-4AD7-84A1-8DA8AE240D81}" name="Note" totalsRowFunction="count" dataDxfId="17" totalsRowDxfId="8"/>
     <tableColumn id="1" xr3:uid="{962D52E2-C6AE-4100-AE8C-DF2E8B9B0615}" name="Ordre" dataDxfId="16" totalsRowDxfId="7"/>
     <tableColumn id="2" xr3:uid="{361935C2-34DD-4D21-A2AB-6BBFCF4F98A2}" name="Nombre" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{C94B1093-5CDB-4631-9DEA-00E6458C936C}" name="Prêt" dataDxfId="9" totalsRowDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{79576F61-0793-4990-BCCE-C22965121196}" name="Fréquence" dataDxfId="14" totalsRowDxfId="4" dataCellStyle="Pourcentage">
+    <tableColumn id="7" xr3:uid="{C94B1093-5CDB-4631-9DEA-00E6458C936C}" name="Prêt" dataDxfId="14" totalsRowDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{79576F61-0793-4990-BCCE-C22965121196}" name="Fréquence" dataDxfId="13" totalsRowDxfId="4" dataCellStyle="Pourcentage">
       <calculatedColumnFormula>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{37230C39-5DD0-41BC-BD2F-700C093E4770}" name="Nombre*Credit" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="3">
+    <tableColumn id="8" xr3:uid="{37230C39-5DD0-41BC-BD2F-700C093E4770}" name="Nombre*Credit" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="3">
       <calculatedColumnFormula>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Credit]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{01749902-06D0-4021-B14B-C7F16B74E64F}" name="Rare?" dataDxfId="12" totalsRowDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{03B71102-410F-4504-A5D5-D6E86877D1E0}" name="Type" dataDxfId="11" totalsRowDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{D6FB2E1D-5A55-46E8-AE05-7C9175F7718F}" name="Credit" dataDxfId="10" totalsRowDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{01749902-06D0-4021-B14B-C7F16B74E64F}" name="Rare?" dataDxfId="11" totalsRowDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{03B71102-410F-4504-A5D5-D6E86877D1E0}" name="Type" dataDxfId="10" totalsRowDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{D6FB2E1D-5A55-46E8-AE05-7C9175F7718F}" name="Credit" dataDxfId="9" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1028,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,7 +1233,9 @@
       <c r="D8" s="1">
         <v>8</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F8" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
         <v>0.08</v>
@@ -1257,7 +1262,9 @@
       <c r="D9" s="1">
         <v>8</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F9" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
         <v>0.08</v>
@@ -1284,7 +1291,9 @@
       <c r="D10" s="1">
         <v>8</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F10" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
         <v>0.08</v>
@@ -1311,7 +1320,9 @@
       <c r="D11" s="1">
         <v>8</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F11" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
         <v>0.08</v>
@@ -1338,7 +1349,9 @@
       <c r="D12" s="1">
         <v>7</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F12" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
         <v>7.0000000000000007E-2</v>
@@ -1365,7 +1378,9 @@
       <c r="D13" s="1">
         <v>7</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F13" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
         <v>7.0000000000000007E-2</v>
@@ -1392,7 +1407,9 @@
       <c r="D14" s="1">
         <v>2</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F14" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
         <v>0.02</v>
@@ -1421,7 +1438,9 @@
       <c r="D15" s="1">
         <v>2</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F15" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
         <v>0.02</v>
@@ -1481,7 +1500,9 @@
       <c r="D17" s="8">
         <v>2</v>
       </c>
-      <c r="E17" s="8"/>
+      <c r="E17" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="F17" s="12">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
         <v>0.02</v>

</xml_diff>

<commit_message>
Fix des cartes à jouer
</commit_message>
<xml_diff>
--- a/docs/Cartes-a-jouer--repartition.xlsx
+++ b/docs/Cartes-a-jouer--repartition.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Documents\GitHub\Donjons-et-Barons\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FF1DB4-3F8D-48C8-ADFD-0F82B8AF1709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BDDA18-50A0-4081-BC07-6DF54DC88CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-9120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-9120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Répartition" sheetId="1" r:id="rId1"/>
+    <sheet name="Présentation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="39">
   <si>
     <t>Type</t>
   </si>
@@ -65,18 +66,12 @@
     <t>Concentrer Troupes</t>
   </si>
   <si>
-    <t>Constuire Donjon</t>
-  </si>
-  <si>
     <t>Chevauchée Lointaine</t>
   </si>
   <si>
     <t>Déconstruire Donjon</t>
   </si>
   <si>
-    <t>Recruter Officier</t>
-  </si>
-  <si>
     <t>Exiler Officier</t>
   </si>
   <si>
@@ -147,6 +142,18 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>Recruter Chevalier</t>
+  </si>
+  <si>
+    <t>Carte</t>
+  </si>
+  <si>
+    <t>Regroupements</t>
+  </si>
+  <si>
+    <t>Construire Donjon</t>
   </si>
 </sst>
 </file>
@@ -180,7 +187,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +212,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA0BE6E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -330,7 +349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -388,6 +407,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -730,6 +770,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFA0BE6E"/>
       <color rgb="FFEBCDE5"/>
     </mruColors>
   </colors>
@@ -1034,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J34"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,19 +1098,19 @@
         <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>6</v>
@@ -1083,7 +1124,7 @@
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -1092,7 +1133,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F3" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
@@ -1112,7 +1153,7 @@
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2">
         <v>2</v>
@@ -1121,7 +1162,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F4" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
@@ -1141,7 +1182,7 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2">
         <v>3</v>
@@ -1150,7 +1191,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F5" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
@@ -1170,7 +1211,7 @@
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2">
         <v>4</v>
@@ -1179,7 +1220,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F6" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
@@ -1199,7 +1240,7 @@
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2">
         <v>5</v>
@@ -1208,7 +1249,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F7" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
@@ -1230,7 +1271,7 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="C8" s="2">
         <v>6</v>
@@ -1239,7 +1280,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F8" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
@@ -1261,7 +1302,7 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2">
         <v>7</v>
@@ -1270,7 +1311,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F9" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
@@ -1292,7 +1333,7 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2">
         <v>8</v>
@@ -1301,7 +1342,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F10" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
@@ -1330,7 +1371,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F11" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
@@ -1359,7 +1400,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F12" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
@@ -1379,7 +1420,7 @@
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" s="2">
         <v>11</v>
@@ -1388,7 +1429,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F13" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
@@ -1408,7 +1449,7 @@
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="2">
         <v>12</v>
@@ -1417,7 +1458,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F14" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
@@ -1437,7 +1478,7 @@
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2">
         <v>13</v>
@@ -1446,7 +1487,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F15" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
@@ -1466,7 +1507,7 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C16" s="2">
         <v>14</v>
@@ -1475,7 +1516,7 @@
         <v>8</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F16" s="11">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
@@ -1495,7 +1536,7 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="7">
         <v>15</v>
@@ -1504,7 +1545,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F17" s="12">
         <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
@@ -1546,11 +1587,11 @@
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -1565,10 +1606,10 @@
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
@@ -1581,10 +1622,10 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="15" t="s">
         <v>30</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
@@ -1597,10 +1638,10 @@
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="19" t="s">
         <v>27</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
@@ -1613,7 +1654,7 @@
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
@@ -1629,4 +1670,255 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E300F5-BB8C-42D4-B150-781935673603}">
+  <dimension ref="B2:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" customWidth="1"/>
+    <col min="4" max="6" width="5.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="18">
+        <v>9</v>
+      </c>
+      <c r="D3" s="25">
+        <f>SUM(C3:C6)</f>
+        <v>36</v>
+      </c>
+      <c r="E3" s="25">
+        <f>SUM(C3:C9)</f>
+        <v>42</v>
+      </c>
+      <c r="F3" s="23">
+        <f>SUM(C3:C17)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="18">
+        <v>9</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="18">
+        <v>9</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="23"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="18">
+        <v>9</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="23"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="18">
+        <v>2</v>
+      </c>
+      <c r="D7" s="25">
+        <f>SUM(C7:C9)</f>
+        <v>6</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="23"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="18">
+        <v>2</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="18">
+        <v>2</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="23"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="20">
+        <v>10</v>
+      </c>
+      <c r="D10" s="22">
+        <f>C10</f>
+        <v>10</v>
+      </c>
+      <c r="E10" s="26">
+        <f>SUM(C10:C17)</f>
+        <v>58</v>
+      </c>
+      <c r="F10" s="23"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="20">
+        <v>8</v>
+      </c>
+      <c r="D11" s="26">
+        <f>SUM(C11:C12)</f>
+        <v>16</v>
+      </c>
+      <c r="E11" s="26"/>
+      <c r="F11" s="23"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="20">
+        <v>8</v>
+      </c>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="23"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="20">
+        <v>8</v>
+      </c>
+      <c r="D13" s="26">
+        <f>SUM(C13:C16)</f>
+        <v>30</v>
+      </c>
+      <c r="E13" s="26"/>
+      <c r="F13" s="23"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="20">
+        <v>7</v>
+      </c>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="23"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="20">
+        <v>7</v>
+      </c>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="23"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="20">
+        <v>8</v>
+      </c>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="23"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="20">
+        <v>2</v>
+      </c>
+      <c r="D17" s="22">
+        <f>C17</f>
+        <v>2</v>
+      </c>
+      <c r="E17" s="26"/>
+      <c r="F17" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="F3:F17"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="E3:E9"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="E10:E17"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C3:C17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D3:E3 D7 E10 D11 D13" formulaRange="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Autres statistiques et idée de la gestion d'action par "Main à Récupération"
</commit_message>
<xml_diff>
--- a/docs/Cartes-a-jouer--repartition.xlsx
+++ b/docs/Cartes-a-jouer--repartition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Documents\GitHub\Donjons-et-Barons\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BDDA18-50A0-4081-BC07-6DF54DC88CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE275B44-DDE6-4D0D-AA21-992D35776967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-9120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
   <si>
     <t>Type</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Construire Donjon</t>
+  </si>
+  <si>
+    <t>Complot à la Cour</t>
   </si>
 </sst>
 </file>
@@ -187,7 +190,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,8 +227,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC28D7C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -344,12 +353,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -414,19 +463,69 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -770,8 +869,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFEBCDE5"/>
+      <color rgb="FFC28D7C"/>
       <color rgb="FFA0BE6E"/>
-      <color rgb="FFEBCDE5"/>
+      <color rgb="FFB5735F"/>
+      <color rgb="FFB57A67"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1674,16 +1776,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E300F5-BB8C-42D4-B150-781935673603}">
-  <dimension ref="B2:F17"/>
+  <dimension ref="B2:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F17"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
     <col min="4" max="6" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1694,217 +1797,188 @@
       <c r="C2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>37</v>
       </c>
       <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="18">
-        <v>9</v>
-      </c>
-      <c r="D3" s="25">
-        <f>SUM(C3:C6)</f>
-        <v>36</v>
-      </c>
-      <c r="E3" s="25">
-        <f>SUM(C3:C9)</f>
-        <v>42</v>
-      </c>
-      <c r="F3" s="23">
-        <f>SUM(C3:C17)</f>
-        <v>100</v>
+        <v>6</v>
+      </c>
+      <c r="D3" s="26">
+        <f>SUM(C3:C5)</f>
+        <v>18</v>
+      </c>
+      <c r="E3" s="27"/>
+      <c r="F3" s="42">
+        <f>SUM(C3:C15)</f>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="18">
-        <v>9</v>
-      </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="23"/>
+        <v>6</v>
+      </c>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="43"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="18">
-        <v>9</v>
-      </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="23"/>
+        <v>6</v>
+      </c>
+      <c r="D5" s="30"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="43"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="18">
-        <v>9</v>
-      </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="23"/>
+      <c r="B6" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="20">
+        <v>2</v>
+      </c>
+      <c r="D6" s="32">
+        <f>SUM(C6:C8)</f>
+        <v>6</v>
+      </c>
+      <c r="E6" s="33">
+        <f>SUM(C6:C11)</f>
+        <v>18</v>
+      </c>
+      <c r="F6" s="43"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="18">
+      <c r="B7" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="20">
         <v>2</v>
       </c>
-      <c r="D7" s="25">
-        <f>SUM(C7:C9)</f>
+      <c r="D7" s="34"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="43"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="20">
+        <v>2</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="43"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="20">
         <v>6</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="23"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="18">
-        <v>2</v>
-      </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="23"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="18">
-        <v>2</v>
-      </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="23"/>
+      <c r="D9" s="20">
+        <f>C9</f>
+        <v>6</v>
+      </c>
+      <c r="E9" s="33"/>
+      <c r="F9" s="43"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="C10" s="20">
-        <v>10</v>
-      </c>
-      <c r="D10" s="22">
-        <f>C10</f>
-        <v>10</v>
-      </c>
-      <c r="E10" s="26">
-        <f>SUM(C10:C17)</f>
-        <v>58</v>
-      </c>
-      <c r="F10" s="23"/>
+        <v>3</v>
+      </c>
+      <c r="D10" s="32">
+        <f>SUM(C10:C11)</f>
+        <v>6</v>
+      </c>
+      <c r="E10" s="33"/>
+      <c r="F10" s="43"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="20" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="20">
-        <v>8</v>
-      </c>
-      <c r="D11" s="26">
-        <f>SUM(C11:C12)</f>
-        <v>16</v>
-      </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="23"/>
+        <v>3</v>
+      </c>
+      <c r="D11" s="35"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="43"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="20">
-        <v>8</v>
-      </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="23"/>
+      <c r="B12" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="18">
+        <v>1</v>
+      </c>
+      <c r="D12" s="36">
+        <f>SUM(C12:C15)</f>
+        <v>4</v>
+      </c>
+      <c r="E12" s="37"/>
+      <c r="F12" s="43"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="20">
-        <v>8</v>
-      </c>
-      <c r="D13" s="26">
-        <f>SUM(C13:C16)</f>
-        <v>30</v>
-      </c>
-      <c r="E13" s="26"/>
-      <c r="F13" s="23"/>
+      <c r="B13" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="18">
+        <v>1</v>
+      </c>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="43"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="20">
-        <v>7</v>
-      </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="23"/>
+      <c r="B14" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="18">
+        <v>1</v>
+      </c>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="43"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="20">
-        <v>7</v>
-      </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="23"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="20">
-        <v>8</v>
-      </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="23"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="20">
-        <v>2</v>
-      </c>
-      <c r="D17" s="22">
-        <f>C17</f>
-        <v>2</v>
-      </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="23"/>
+      <c r="B15" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="18">
+        <v>1</v>
+      </c>
+      <c r="D15" s="40"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="F3:F17"/>
+  <mergeCells count="7">
     <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="E3:E9"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="E10:E17"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E6:E11"/>
+    <mergeCell ref="F3:F15"/>
+    <mergeCell ref="D3:E5"/>
+    <mergeCell ref="D12:E15"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:C17">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="C3:C5">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1915,10 +1989,90 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C6:C8">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:C15">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C15">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D3:E3 D7 E10 D11 D13" formulaRange="1"/>
+    <ignoredError sqref="D6:E6 D10 D12 D3" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>